<commit_message>
Ajouts de tests pitch schifter
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Revue2/Plan_test_integration_Revue2.xlsx
+++ b/Documentation/Tests/Revue2/Plan_test_integration_Revue2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olaberge\Documents\S5\Projet S5\Repo_Projet_S5\Remises\Revue2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olaberge\Documents\S5\Projet S5\Repo_Projet_S5\Documentation\Tests\Revue2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3399F6CA-878F-4C68-BA4E-00DEDE61B4D4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD6BDAC-E1C5-459B-84DA-AF7E7E0A35D5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" activeTab="2" xr2:uid="{73256A17-FE39-444F-BF69-663F23F71EB5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="2" xr2:uid="{73256A17-FE39-444F-BF69-663F23F71EB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Gabarit" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="134">
   <si>
     <t>Personne responsable:</t>
   </si>
@@ -183,12 +183,6 @@
     <t>3 Mars 2018</t>
   </si>
   <si>
-    <t>Revue 1</t>
-  </si>
-  <si>
-    <t>Harmoniseur:</t>
-  </si>
-  <si>
     <t>Égaliseur:</t>
   </si>
   <si>
@@ -375,13 +369,7 @@
     <t>2.10.3</t>
   </si>
   <si>
-    <t>Entrée: Sinus avec 50 harmoniques avec 50 amplitudes différentes</t>
-  </si>
-  <si>
     <t>maxFFT et reconstruction signal</t>
-  </si>
-  <si>
-    <t>Sinus avec 50 harmoniques avec 50 amplitudes différentes dont les 32 harmoniques les plus importantes sont amplifié comparé au signal original</t>
   </si>
   <si>
     <t>Autocorrelation et 0.9*MAX(1) (Deuxième canal):</t>
@@ -442,6 +430,15 @@
     <t>Signal de démarrage: Signal de 
 1 kHz, 1V
 Signal de démarrage pré-enregistré: Signal de 2 kHz, 1V</t>
+  </si>
+  <si>
+    <t>Pitch Schifter:</t>
+  </si>
+  <si>
+    <t>Revue 2</t>
+  </si>
+  <si>
+    <t>Entrée: Signal peut-importe</t>
   </si>
 </sst>
 </file>
@@ -1276,6 +1273,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1305,72 +1374,111 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1380,48 +1488,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1431,89 +1497,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1851,16 +1848,16 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
-      <c r="F2" s="38" t="s">
+      <c r="C2" s="60"/>
+      <c r="D2" s="61"/>
+      <c r="F2" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="65"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1869,16 +1866,16 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="F3" s="42" t="s">
+      <c r="C3" s="68"/>
+      <c r="D3" s="69"/>
+      <c r="F3" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="45"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="50"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -1887,22 +1884,22 @@
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="52" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="56" t="s">
+      <c r="F5" s="40"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="57"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41"/>
       <c r="L5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1917,181 +1914,181 @@
       <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B6" s="58"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="62"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="60"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="54"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
-      <c r="O6" s="33"/>
+      <c r="O6" s="57"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>2</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="50"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="56"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="O7" s="34"/>
+      <c r="O7" s="58"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="50"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="56"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="O8" s="34"/>
+      <c r="O8" s="58"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>4</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="50"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="56"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="O9" s="34"/>
+      <c r="O9" s="58"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>5</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="50"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="56"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="O10" s="34"/>
+      <c r="O10" s="58"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>6</v>
       </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="50"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="56"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="O11" s="34"/>
+      <c r="O11" s="58"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="48"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="50"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="56"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="O12" s="34"/>
+      <c r="O12" s="58"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>8</v>
       </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="50"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="56"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="O13" s="34"/>
+      <c r="O13" s="58"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>9</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="50"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="56"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="O14" s="34"/>
+      <c r="O14" s="58"/>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="8">
         <v>10</v>
       </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="45"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="50"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="O15" s="35"/>
+      <c r="O15" s="59"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
@@ -2106,6 +2103,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="O6:O15"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E7:G7"/>
@@ -2122,30 +2143,6 @@
     <mergeCell ref="H14:K14"/>
     <mergeCell ref="E8:G8"/>
     <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="O6:O15"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2174,20 +2171,20 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="F2" s="38" t="s">
+      <c r="D2" s="61"/>
+      <c r="F2" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40" t="s">
+      <c r="G2" s="63"/>
+      <c r="H2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="65"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2196,23 +2193,23 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="68">
         <v>1</v>
       </c>
-      <c r="D3" s="47"/>
+      <c r="D3" s="69"/>
       <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44" t="s">
+      <c r="G3" s="67"/>
+      <c r="H3" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="45"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="50"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -2221,22 +2218,22 @@
       <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36" t="s">
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36" t="s">
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
       <c r="L5" s="16" t="s">
         <v>7</v>
       </c>
@@ -2248,41 +2245,41 @@
       <c r="A6" s="22">
         <v>1</v>
       </c>
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-      <c r="M6" s="94"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="M6" s="75"/>
     </row>
     <row r="7" spans="1:14" ht="72" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="77" t="s">
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78"/>
-      <c r="H7" s="86" t="s">
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="88"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="90"/>
       <c r="L7" s="20" t="s">
         <v>18</v>
       </c>
@@ -2292,22 +2289,22 @@
       <c r="A8" s="24">
         <v>1.2</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="101" t="s">
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="102"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="86" t="s">
+      <c r="F8" s="87"/>
+      <c r="G8" s="87"/>
+      <c r="H8" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="87"/>
-      <c r="J8" s="87"/>
-      <c r="K8" s="88"/>
+      <c r="I8" s="89"/>
+      <c r="J8" s="89"/>
+      <c r="K8" s="90"/>
       <c r="L8" s="18" t="s">
         <v>18</v>
       </c>
@@ -2317,22 +2314,22 @@
       <c r="A9" s="25">
         <v>1.3</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="81" t="s">
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="86" t="s">
+      <c r="F9" s="98"/>
+      <c r="G9" s="98"/>
+      <c r="H9" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="87"/>
-      <c r="J9" s="87"/>
-      <c r="K9" s="88"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="89"/>
+      <c r="K9" s="90"/>
       <c r="L9" s="19" t="s">
         <v>18</v>
       </c>
@@ -2342,41 +2339,41 @@
       <c r="A10" s="22">
         <v>2</v>
       </c>
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93"/>
-      <c r="E10" s="93"/>
-      <c r="F10" s="93"/>
-      <c r="G10" s="93"/>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="93"/>
-      <c r="M10" s="94"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="75"/>
     </row>
     <row r="11" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23">
         <v>2.1</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="77" t="s">
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="86" t="s">
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="87"/>
-      <c r="J11" s="87"/>
-      <c r="K11" s="88"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="90"/>
       <c r="L11" s="20" t="s">
         <v>19</v>
       </c>
@@ -2386,22 +2383,22 @@
       <c r="A12" s="24">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="79" t="s">
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="66" t="s">
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="68"/>
+      <c r="I12" s="104"/>
+      <c r="J12" s="104"/>
+      <c r="K12" s="105"/>
       <c r="L12" s="18" t="s">
         <v>19</v>
       </c>
@@ -2413,22 +2410,22 @@
       <c r="A13" s="25">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="81" t="s">
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="83" t="s">
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="84"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="85"/>
+      <c r="I13" s="107"/>
+      <c r="J13" s="107"/>
+      <c r="K13" s="108"/>
       <c r="L13" s="19" t="s">
         <v>19</v>
       </c>
@@ -2438,41 +2435,41 @@
       <c r="A14" s="22">
         <v>3</v>
       </c>
-      <c r="B14" s="93" t="s">
+      <c r="B14" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="93"/>
-      <c r="K14" s="93"/>
-      <c r="L14" s="93"/>
-      <c r="M14" s="94"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="74"/>
+      <c r="M14" s="75"/>
     </row>
     <row r="15" spans="1:14" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23">
         <v>3.1</v>
       </c>
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="89" t="s">
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="86" t="s">
+      <c r="F15" s="100"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="87"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="88"/>
+      <c r="I15" s="89"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="90"/>
       <c r="L15" s="20" t="s">
         <v>19</v>
       </c>
@@ -2482,22 +2479,22 @@
       <c r="A16" s="24">
         <v>3.2</v>
       </c>
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="74"/>
-      <c r="D16" s="74"/>
-      <c r="E16" s="79" t="s">
+      <c r="C16" s="85"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="80"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="66" t="s">
+      <c r="F16" s="102"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="68"/>
+      <c r="I16" s="104"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="105"/>
       <c r="L16" s="18" t="s">
         <v>19</v>
       </c>
@@ -2509,22 +2506,22 @@
       <c r="A17" s="25">
         <v>3.3</v>
       </c>
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="81" t="s">
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="82"/>
-      <c r="G17" s="82"/>
-      <c r="H17" s="83" t="s">
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="84"/>
-      <c r="J17" s="84"/>
-      <c r="K17" s="85"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="107"/>
+      <c r="K17" s="108"/>
       <c r="L17" s="19" t="s">
         <v>19</v>
       </c>
@@ -2534,41 +2531,41 @@
       <c r="A18" s="22">
         <v>4</v>
       </c>
-      <c r="B18" s="93" t="s">
+      <c r="B18" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="93"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="93"/>
-      <c r="L18" s="93"/>
-      <c r="M18" s="94"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="74"/>
+      <c r="K18" s="74"/>
+      <c r="L18" s="74"/>
+      <c r="M18" s="75"/>
     </row>
     <row r="19" spans="1:13" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="26">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65" t="s">
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="69" t="s">
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="70"/>
-      <c r="J19" s="70"/>
-      <c r="K19" s="70"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77"/>
       <c r="L19" s="27" t="s">
         <v>19</v>
       </c>
@@ -2580,22 +2577,22 @@
       <c r="A20" s="26">
         <v>4.3</v>
       </c>
-      <c r="B20" s="92" t="s">
+      <c r="B20" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="95" t="s">
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="96"/>
-      <c r="G20" s="97"/>
-      <c r="H20" s="98" t="s">
+      <c r="F20" s="79"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="99"/>
-      <c r="J20" s="99"/>
-      <c r="K20" s="100"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
+      <c r="K20" s="83"/>
       <c r="L20" s="27" t="s">
         <v>19</v>
       </c>
@@ -2607,22 +2604,22 @@
       <c r="A21" s="26">
         <v>4.2</v>
       </c>
-      <c r="B21" s="92" t="s">
+      <c r="B21" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65" t="s">
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="69" t="s">
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="I21" s="70"/>
-      <c r="J21" s="70"/>
-      <c r="K21" s="70"/>
+      <c r="I21" s="77"/>
+      <c r="J21" s="77"/>
+      <c r="K21" s="77"/>
       <c r="L21" s="27" t="s">
         <v>19</v>
       </c>
@@ -2652,6 +2649,39 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="H21:K21"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:K3"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:K5"/>
@@ -2668,39 +2698,6 @@
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:G8"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2710,8 +2707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAD95B45-4342-44B1-A40B-F30FB3A286B9}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2727,20 +2724,20 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="F2" s="38" t="s">
+      <c r="D2" s="61"/>
+      <c r="F2" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40" t="s">
+      <c r="G2" s="63"/>
+      <c r="H2" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="41"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="65"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2749,23 +2746,23 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="46">
+      <c r="C3" s="68">
         <v>1</v>
       </c>
-      <c r="D3" s="47"/>
+      <c r="D3" s="69"/>
       <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="45"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="50"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -2773,22 +2770,22 @@
       <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49" t="s">
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49" t="s">
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
       <c r="L5" s="32" t="s">
         <v>7</v>
       </c>
@@ -2797,642 +2794,640 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="111">
+      <c r="A6" s="37">
         <v>1</v>
       </c>
-      <c r="B6" s="112" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="112"/>
-      <c r="L6" s="112"/>
-      <c r="M6" s="112"/>
+      <c r="B6" s="113" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="113"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
+      <c r="G6" s="113"/>
+      <c r="H6" s="113"/>
+      <c r="I6" s="113"/>
+      <c r="J6" s="113"/>
+      <c r="K6" s="113"/>
+      <c r="L6" s="113"/>
+      <c r="M6" s="113"/>
     </row>
     <row r="7" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="105" t="s">
-        <v>115</v>
-      </c>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="105"/>
-      <c r="I7" s="105"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="105"/>
-      <c r="L7" s="105"/>
-      <c r="M7" s="105"/>
+      <c r="B7" s="112" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="112"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="112"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="112"/>
+      <c r="J7" s="112"/>
+      <c r="K7" s="112"/>
+      <c r="L7" s="112"/>
+      <c r="M7" s="112"/>
     </row>
     <row r="8" spans="1:14" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="105" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" s="105"/>
-      <c r="G8" s="105"/>
-      <c r="H8" s="105"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="105"/>
-      <c r="L8" s="107"/>
-      <c r="M8" s="107"/>
+        <v>54</v>
+      </c>
+      <c r="B8" s="112" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="112"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="112"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="112"/>
+      <c r="K8" s="112"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
     </row>
     <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="111">
+      <c r="A9" s="37">
         <v>2</v>
       </c>
-      <c r="B9" s="112" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="112"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="112"/>
-      <c r="I9" s="112"/>
-      <c r="J9" s="112"/>
-      <c r="K9" s="112"/>
-      <c r="L9" s="112"/>
-      <c r="M9" s="112"/>
+      <c r="B9" s="113" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="113"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="113"/>
+      <c r="K9" s="113"/>
+      <c r="L9" s="113"/>
+      <c r="M9" s="113"/>
     </row>
     <row r="10" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18">
         <v>2.1</v>
       </c>
-      <c r="B10" s="105" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="105"/>
-      <c r="J10" s="105"/>
-      <c r="K10" s="105"/>
-      <c r="L10" s="105"/>
-      <c r="M10" s="105"/>
+      <c r="B10" s="112" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="112"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="112"/>
+      <c r="G10" s="112"/>
+      <c r="H10" s="112"/>
+      <c r="I10" s="112"/>
+      <c r="J10" s="112"/>
+      <c r="K10" s="112"/>
+      <c r="L10" s="112"/>
+      <c r="M10" s="112"/>
     </row>
     <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="105" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="105"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="108"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="103"/>
-      <c r="K11" s="109"/>
-      <c r="L11" s="104"/>
-      <c r="M11" s="104"/>
+        <v>55</v>
+      </c>
+      <c r="B11" s="112" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="112"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="112"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="110"/>
+      <c r="J11" s="110"/>
+      <c r="K11" s="111"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
     </row>
     <row r="12" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="105" t="s">
-        <v>119</v>
-      </c>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="105" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="103"/>
-      <c r="J12" s="103"/>
-      <c r="K12" s="109"/>
-      <c r="L12" s="104"/>
-      <c r="M12" s="104"/>
+        <v>56</v>
+      </c>
+      <c r="B12" s="112" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="112"/>
+      <c r="G12" s="112"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="110"/>
+      <c r="J12" s="110"/>
+      <c r="K12" s="111"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33"/>
     </row>
     <row r="13" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B13" s="105" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="105"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105"/>
+      <c r="B13" s="112" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="112"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="112"/>
     </row>
     <row r="14" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="105" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105" t="s">
-        <v>93</v>
-      </c>
-      <c r="F14" s="105"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="108"/>
-      <c r="I14" s="103"/>
-      <c r="J14" s="103"/>
-      <c r="K14" s="109"/>
-      <c r="L14" s="104"/>
-      <c r="M14" s="104"/>
+        <v>57</v>
+      </c>
+      <c r="B14" s="112" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="112"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="112" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="112"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="110"/>
+      <c r="K14" s="111"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
     </row>
     <row r="15" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="105" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="103"/>
-      <c r="K15" s="109"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
+        <v>58</v>
+      </c>
+      <c r="B15" s="112" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="112"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="110"/>
+      <c r="J15" s="110"/>
+      <c r="K15" s="111"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
     </row>
     <row r="16" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B16" s="105" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="105"/>
-      <c r="K16" s="105"/>
-      <c r="L16" s="105"/>
-      <c r="M16" s="105"/>
+      <c r="B16" s="112" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="112"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
+      <c r="G16" s="112"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="112"/>
+      <c r="J16" s="112"/>
+      <c r="K16" s="112"/>
+      <c r="L16" s="112"/>
+      <c r="M16" s="112"/>
     </row>
     <row r="17" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="105" t="s">
-        <v>120</v>
-      </c>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="105" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="103"/>
-      <c r="J17" s="103"/>
-      <c r="K17" s="109"/>
-      <c r="L17" s="104"/>
-      <c r="M17" s="104"/>
+        <v>59</v>
+      </c>
+      <c r="B17" s="112" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="112"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="112"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="110"/>
+      <c r="K17" s="111"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
     </row>
     <row r="18" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="105" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" s="105"/>
-      <c r="D18" s="105"/>
-      <c r="E18" s="105" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="108"/>
-      <c r="I18" s="103"/>
-      <c r="J18" s="103"/>
-      <c r="K18" s="109"/>
-      <c r="L18" s="104"/>
-      <c r="M18" s="104"/>
+        <v>60</v>
+      </c>
+      <c r="B18" s="112" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="110"/>
+      <c r="J18" s="110"/>
+      <c r="K18" s="111"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
     </row>
     <row r="19" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="105" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="105"/>
-      <c r="D19" s="105"/>
-      <c r="E19" s="105" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="105"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="103"/>
-      <c r="J19" s="103"/>
-      <c r="K19" s="109"/>
-      <c r="L19" s="104"/>
-      <c r="M19" s="104"/>
+        <v>72</v>
+      </c>
+      <c r="B19" s="112" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="112"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="112"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="110"/>
+      <c r="J19" s="110"/>
+      <c r="K19" s="111"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
     </row>
     <row r="20" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="105" t="s">
-        <v>122</v>
-      </c>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="108" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="103"/>
-      <c r="G20" s="109"/>
-      <c r="H20" s="108"/>
-      <c r="I20" s="103"/>
-      <c r="J20" s="103"/>
-      <c r="K20" s="109"/>
-      <c r="L20" s="104"/>
-      <c r="M20" s="104"/>
+        <v>73</v>
+      </c>
+      <c r="B20" s="112" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="112"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="109" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="110"/>
+      <c r="G20" s="111"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="110"/>
+      <c r="K20" s="111"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
     </row>
     <row r="21" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18">
         <v>2.4</v>
       </c>
-      <c r="B21" s="105" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="105"/>
-      <c r="I21" s="105"/>
-      <c r="J21" s="105"/>
-      <c r="K21" s="105"/>
-      <c r="L21" s="105"/>
-      <c r="M21" s="105"/>
+      <c r="B21" s="112" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
+      <c r="F21" s="112"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="112"/>
+      <c r="L21" s="112"/>
+      <c r="M21" s="112"/>
     </row>
     <row r="22" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="105" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22" s="105"/>
-      <c r="D22" s="105"/>
-      <c r="E22" s="105" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="105"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="108"/>
-      <c r="I22" s="103"/>
-      <c r="J22" s="103"/>
-      <c r="K22" s="109"/>
-      <c r="L22" s="104"/>
-      <c r="M22" s="104"/>
+        <v>61</v>
+      </c>
+      <c r="B22" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="112"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="112" t="s">
+        <v>86</v>
+      </c>
+      <c r="F22" s="112"/>
+      <c r="G22" s="112"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="110"/>
+      <c r="J22" s="110"/>
+      <c r="K22" s="111"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
     </row>
     <row r="23" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="108" t="s">
-        <v>124</v>
-      </c>
-      <c r="C23" s="103"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="108" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="103"/>
-      <c r="G23" s="109"/>
-      <c r="H23" s="108"/>
-      <c r="I23" s="103"/>
-      <c r="J23" s="103"/>
-      <c r="K23" s="109"/>
-      <c r="L23" s="104"/>
-      <c r="M23" s="104"/>
+        <v>62</v>
+      </c>
+      <c r="B23" s="109" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="110"/>
+      <c r="D23" s="111"/>
+      <c r="E23" s="109" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="110"/>
+      <c r="G23" s="111"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="110"/>
+      <c r="J23" s="110"/>
+      <c r="K23" s="111"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
     </row>
     <row r="24" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" s="108" t="s">
-        <v>125</v>
-      </c>
-      <c r="C24" s="103"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="108" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="103"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="108"/>
-      <c r="I24" s="103"/>
-      <c r="J24" s="103"/>
-      <c r="K24" s="109"/>
-      <c r="L24" s="104"/>
-      <c r="M24" s="104"/>
+        <v>82</v>
+      </c>
+      <c r="B24" s="109" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="110"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="109" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="110"/>
+      <c r="G24" s="111"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="110"/>
+      <c r="J24" s="110"/>
+      <c r="K24" s="111"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
     </row>
     <row r="25" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="B25" s="108" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" s="103"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="108" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" s="103"/>
-      <c r="G25" s="109"/>
-      <c r="H25" s="108"/>
-      <c r="I25" s="103"/>
-      <c r="J25" s="103"/>
-      <c r="K25" s="109"/>
-      <c r="L25" s="104"/>
-      <c r="M25" s="104"/>
+        <v>102</v>
+      </c>
+      <c r="B25" s="109" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="110"/>
+      <c r="D25" s="111"/>
+      <c r="E25" s="109" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="110"/>
+      <c r="G25" s="111"/>
+      <c r="H25" s="109"/>
+      <c r="I25" s="110"/>
+      <c r="J25" s="110"/>
+      <c r="K25" s="111"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
     </row>
     <row r="26" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18">
         <v>2.5</v>
       </c>
-      <c r="B26" s="108" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="103"/>
-      <c r="D26" s="103"/>
-      <c r="E26" s="103"/>
-      <c r="F26" s="103"/>
-      <c r="G26" s="103"/>
-      <c r="H26" s="103"/>
-      <c r="I26" s="103"/>
-      <c r="J26" s="103"/>
-      <c r="K26" s="103"/>
-      <c r="L26" s="103"/>
-      <c r="M26" s="109"/>
+      <c r="B26" s="109" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="110"/>
+      <c r="G26" s="110"/>
+      <c r="H26" s="110"/>
+      <c r="I26" s="110"/>
+      <c r="J26" s="110"/>
+      <c r="K26" s="110"/>
+      <c r="L26" s="110"/>
+      <c r="M26" s="111"/>
     </row>
     <row r="27" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" s="105" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27" s="105"/>
-      <c r="D27" s="105"/>
-      <c r="E27" s="105" t="s">
-        <v>94</v>
-      </c>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
-      <c r="H27" s="108"/>
-      <c r="I27" s="103"/>
-      <c r="J27" s="103"/>
-      <c r="K27" s="109"/>
-      <c r="L27" s="104"/>
-      <c r="M27" s="104"/>
+        <v>63</v>
+      </c>
+      <c r="B27" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="112"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="112" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="112"/>
+      <c r="G27" s="112"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="110"/>
+      <c r="J27" s="110"/>
+      <c r="K27" s="111"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
     </row>
     <row r="28" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="108" t="s">
-        <v>124</v>
-      </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="109"/>
-      <c r="E28" s="108" t="s">
-        <v>101</v>
-      </c>
-      <c r="F28" s="103"/>
-      <c r="G28" s="109"/>
-      <c r="H28" s="108"/>
-      <c r="I28" s="103"/>
-      <c r="J28" s="103"/>
-      <c r="K28" s="109"/>
-      <c r="L28" s="104"/>
-      <c r="M28" s="104"/>
+        <v>64</v>
+      </c>
+      <c r="B28" s="109" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="110"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="109" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="110"/>
+      <c r="G28" s="111"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="110"/>
+      <c r="J28" s="110"/>
+      <c r="K28" s="111"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
     </row>
     <row r="29" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="108" t="s">
-        <v>125</v>
-      </c>
-      <c r="C29" s="103"/>
-      <c r="D29" s="109"/>
-      <c r="E29" s="108" t="s">
-        <v>80</v>
-      </c>
-      <c r="F29" s="103"/>
-      <c r="G29" s="109"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="103"/>
-      <c r="J29" s="103"/>
-      <c r="K29" s="109"/>
-      <c r="L29" s="104"/>
-      <c r="M29" s="104"/>
+        <v>74</v>
+      </c>
+      <c r="B29" s="109" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="110"/>
+      <c r="D29" s="111"/>
+      <c r="E29" s="109" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="110"/>
+      <c r="G29" s="111"/>
+      <c r="H29" s="109"/>
+      <c r="I29" s="110"/>
+      <c r="J29" s="110"/>
+      <c r="K29" s="111"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
     </row>
     <row r="30" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="108" t="s">
-        <v>126</v>
-      </c>
-      <c r="C30" s="103"/>
-      <c r="D30" s="109"/>
-      <c r="E30" s="108" t="s">
-        <v>80</v>
-      </c>
-      <c r="F30" s="103"/>
-      <c r="G30" s="109"/>
-      <c r="H30" s="108"/>
-      <c r="I30" s="103"/>
-      <c r="J30" s="103"/>
-      <c r="K30" s="109"/>
-      <c r="L30" s="104"/>
-      <c r="M30" s="104"/>
+        <v>75</v>
+      </c>
+      <c r="B30" s="109" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="110"/>
+      <c r="D30" s="111"/>
+      <c r="E30" s="109" t="s">
+        <v>78</v>
+      </c>
+      <c r="F30" s="110"/>
+      <c r="G30" s="111"/>
+      <c r="H30" s="109"/>
+      <c r="I30" s="110"/>
+      <c r="J30" s="110"/>
+      <c r="K30" s="111"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
     </row>
     <row r="31" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18">
         <v>2.6</v>
       </c>
-      <c r="B31" s="105" t="s">
-        <v>102</v>
-      </c>
-      <c r="C31" s="105"/>
-      <c r="D31" s="105"/>
-      <c r="E31" s="105"/>
-      <c r="F31" s="105"/>
-      <c r="G31" s="105"/>
-      <c r="H31" s="105"/>
-      <c r="I31" s="105"/>
-      <c r="J31" s="105"/>
-      <c r="K31" s="105"/>
-      <c r="L31" s="105"/>
-      <c r="M31" s="105"/>
+      <c r="B31" s="112" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="112"/>
+      <c r="D31" s="112"/>
+      <c r="E31" s="112"/>
+      <c r="F31" s="112"/>
+      <c r="G31" s="112"/>
+      <c r="H31" s="112"/>
+      <c r="I31" s="112"/>
+      <c r="J31" s="112"/>
+      <c r="K31" s="112"/>
+      <c r="L31" s="112"/>
+      <c r="M31" s="112"/>
     </row>
     <row r="32" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="105" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" s="105"/>
-      <c r="D32" s="105"/>
-      <c r="E32" s="105" t="s">
-        <v>89</v>
-      </c>
-      <c r="F32" s="105"/>
-      <c r="G32" s="105"/>
-      <c r="H32" s="108"/>
-      <c r="I32" s="103"/>
-      <c r="J32" s="103"/>
-      <c r="K32" s="109"/>
-      <c r="L32" s="104"/>
-      <c r="M32" s="104"/>
+        <v>65</v>
+      </c>
+      <c r="B32" s="112" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="112"/>
+      <c r="D32" s="112"/>
+      <c r="E32" s="112" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" s="112"/>
+      <c r="G32" s="112"/>
+      <c r="H32" s="109"/>
+      <c r="I32" s="110"/>
+      <c r="J32" s="110"/>
+      <c r="K32" s="111"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
     </row>
     <row r="33" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="105" t="s">
-        <v>125</v>
-      </c>
-      <c r="C33" s="105"/>
-      <c r="D33" s="105"/>
-      <c r="E33" s="108" t="s">
-        <v>80</v>
-      </c>
-      <c r="F33" s="103"/>
-      <c r="G33" s="109"/>
-      <c r="H33" s="108"/>
-      <c r="I33" s="103"/>
-      <c r="J33" s="103"/>
-      <c r="K33" s="109"/>
-      <c r="L33" s="104"/>
-      <c r="M33" s="104"/>
+        <v>66</v>
+      </c>
+      <c r="B33" s="112" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="112"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="109" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="110"/>
+      <c r="G33" s="111"/>
+      <c r="H33" s="109"/>
+      <c r="I33" s="110"/>
+      <c r="J33" s="110"/>
+      <c r="K33" s="111"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
     </row>
     <row r="34" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="18">
         <v>2.7</v>
       </c>
-      <c r="B34" s="105" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="105"/>
-      <c r="D34" s="105"/>
-      <c r="E34" s="105"/>
-      <c r="F34" s="105"/>
-      <c r="G34" s="105"/>
-      <c r="H34" s="105"/>
-      <c r="I34" s="105"/>
-      <c r="J34" s="105"/>
-      <c r="K34" s="105"/>
-      <c r="L34" s="105"/>
-      <c r="M34" s="105"/>
+      <c r="B34" s="112" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="112"/>
+      <c r="H34" s="112"/>
+      <c r="I34" s="112"/>
+      <c r="J34" s="112"/>
+      <c r="K34" s="112"/>
+      <c r="L34" s="112"/>
+      <c r="M34" s="112"/>
     </row>
     <row r="35" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="105" t="s">
-        <v>127</v>
-      </c>
-      <c r="C35" s="105"/>
-      <c r="D35" s="105"/>
-      <c r="E35" s="105" t="s">
-        <v>95</v>
-      </c>
-      <c r="F35" s="105"/>
-      <c r="G35" s="105"/>
-      <c r="H35" s="108"/>
-      <c r="I35" s="103"/>
-      <c r="J35" s="103"/>
-      <c r="K35" s="109"/>
-      <c r="L35" s="104"/>
-      <c r="M35" s="104"/>
+        <v>88</v>
+      </c>
+      <c r="B35" s="112" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" s="112"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="112" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35" s="112"/>
+      <c r="G35" s="112"/>
+      <c r="H35" s="109"/>
+      <c r="I35" s="110"/>
+      <c r="J35" s="110"/>
+      <c r="K35" s="111"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
     </row>
     <row r="36" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B36" s="105" t="s">
-        <v>125</v>
-      </c>
-      <c r="C36" s="105"/>
-      <c r="D36" s="105"/>
-      <c r="E36" s="108" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="112" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="112"/>
+      <c r="D36" s="112"/>
+      <c r="E36" s="109" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" s="110"/>
+      <c r="G36" s="111"/>
+      <c r="H36" s="109"/>
+      <c r="I36" s="110"/>
+      <c r="J36" s="110"/>
+      <c r="K36" s="111"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+    </row>
+    <row r="37" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="38">
+        <v>2.8</v>
+      </c>
+      <c r="B37" s="114" t="s">
         <v>80</v>
-      </c>
-      <c r="F36" s="103"/>
-      <c r="G36" s="109"/>
-      <c r="H36" s="108"/>
-      <c r="I36" s="103"/>
-      <c r="J36" s="103"/>
-      <c r="K36" s="109"/>
-      <c r="L36" s="104"/>
-      <c r="M36" s="104"/>
-    </row>
-    <row r="37" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="113">
-        <v>2.8</v>
-      </c>
-      <c r="B37" s="114" t="s">
-        <v>82</v>
       </c>
       <c r="C37" s="114"/>
       <c r="D37" s="114"/>
@@ -3448,405 +3443,405 @@
     </row>
     <row r="38" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B38" s="105" t="s">
-        <v>128</v>
-      </c>
-      <c r="C38" s="105"/>
-      <c r="D38" s="105"/>
-      <c r="E38" s="105" t="s">
-        <v>83</v>
-      </c>
-      <c r="F38" s="105"/>
-      <c r="G38" s="105"/>
-      <c r="H38" s="108"/>
-      <c r="I38" s="103"/>
-      <c r="J38" s="103"/>
-      <c r="K38" s="109"/>
-      <c r="L38" s="104"/>
-      <c r="M38" s="104"/>
+        <v>103</v>
+      </c>
+      <c r="B38" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="112"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="112" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="112"/>
+      <c r="G38" s="112"/>
+      <c r="H38" s="109"/>
+      <c r="I38" s="110"/>
+      <c r="J38" s="110"/>
+      <c r="K38" s="111"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
     </row>
     <row r="39" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="B39" s="105" t="s">
-        <v>123</v>
-      </c>
-      <c r="C39" s="105"/>
-      <c r="D39" s="105"/>
-      <c r="E39" s="105" t="s">
-        <v>78</v>
-      </c>
-      <c r="F39" s="105"/>
-      <c r="G39" s="105"/>
-      <c r="H39" s="108"/>
-      <c r="I39" s="103"/>
-      <c r="J39" s="103"/>
-      <c r="K39" s="109"/>
-      <c r="L39" s="104"/>
-      <c r="M39" s="104"/>
+        <v>104</v>
+      </c>
+      <c r="B39" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="112"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="112" t="s">
+        <v>76</v>
+      </c>
+      <c r="F39" s="112"/>
+      <c r="G39" s="112"/>
+      <c r="H39" s="109"/>
+      <c r="I39" s="110"/>
+      <c r="J39" s="110"/>
+      <c r="K39" s="111"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
     </row>
     <row r="40" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B40" s="105" t="s">
-        <v>127</v>
-      </c>
-      <c r="C40" s="105"/>
-      <c r="D40" s="105"/>
-      <c r="E40" s="105" t="s">
-        <v>85</v>
-      </c>
-      <c r="F40" s="105"/>
-      <c r="G40" s="105"/>
-      <c r="H40" s="108"/>
-      <c r="I40" s="103"/>
-      <c r="J40" s="103"/>
-      <c r="K40" s="109"/>
-      <c r="L40" s="104"/>
-      <c r="M40" s="104"/>
+        <v>105</v>
+      </c>
+      <c r="B40" s="112" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="112"/>
+      <c r="D40" s="112"/>
+      <c r="E40" s="112" t="s">
+        <v>83</v>
+      </c>
+      <c r="F40" s="112"/>
+      <c r="G40" s="112"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="110"/>
+      <c r="J40" s="110"/>
+      <c r="K40" s="111"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
     </row>
     <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="18">
         <v>2.9</v>
       </c>
-      <c r="B41" s="105" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="105"/>
-      <c r="D41" s="105"/>
-      <c r="E41" s="105"/>
-      <c r="F41" s="105"/>
-      <c r="G41" s="105"/>
-      <c r="H41" s="105"/>
-      <c r="I41" s="105"/>
-      <c r="J41" s="105"/>
-      <c r="K41" s="105"/>
-      <c r="L41" s="105"/>
-      <c r="M41" s="105"/>
+      <c r="B41" s="112" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="112"/>
+      <c r="G41" s="112"/>
+      <c r="H41" s="112"/>
+      <c r="I41" s="112"/>
+      <c r="J41" s="112"/>
+      <c r="K41" s="112"/>
+      <c r="L41" s="112"/>
+      <c r="M41" s="112"/>
     </row>
     <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="B42" s="105" t="s">
-        <v>128</v>
-      </c>
-      <c r="C42" s="105"/>
-      <c r="D42" s="105"/>
-      <c r="E42" s="108" t="s">
-        <v>87</v>
-      </c>
-      <c r="F42" s="103"/>
-      <c r="G42" s="109"/>
-      <c r="H42" s="108"/>
-      <c r="I42" s="103"/>
-      <c r="J42" s="103"/>
-      <c r="K42" s="109"/>
-      <c r="L42" s="104"/>
-      <c r="M42" s="104"/>
+        <v>106</v>
+      </c>
+      <c r="B42" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="110"/>
+      <c r="G42" s="111"/>
+      <c r="H42" s="109"/>
+      <c r="I42" s="110"/>
+      <c r="J42" s="110"/>
+      <c r="K42" s="111"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
     </row>
     <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" s="105" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" s="105"/>
-      <c r="D43" s="105"/>
-      <c r="E43" s="105" t="s">
-        <v>88</v>
-      </c>
-      <c r="F43" s="105"/>
-      <c r="G43" s="105"/>
-      <c r="H43" s="108"/>
-      <c r="I43" s="103"/>
-      <c r="J43" s="103"/>
-      <c r="K43" s="109"/>
-      <c r="L43" s="104"/>
-      <c r="M43" s="104"/>
+        <v>107</v>
+      </c>
+      <c r="B43" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="112"/>
+      <c r="D43" s="112"/>
+      <c r="E43" s="112" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="112"/>
+      <c r="G43" s="112"/>
+      <c r="H43" s="109"/>
+      <c r="I43" s="110"/>
+      <c r="J43" s="110"/>
+      <c r="K43" s="111"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
     </row>
     <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="B44" s="105" t="s">
-        <v>127</v>
-      </c>
-      <c r="C44" s="105"/>
-      <c r="D44" s="105"/>
-      <c r="E44" s="108" t="s">
-        <v>89</v>
-      </c>
-      <c r="F44" s="103"/>
-      <c r="G44" s="109"/>
-      <c r="H44" s="108"/>
-      <c r="I44" s="103"/>
-      <c r="J44" s="103"/>
-      <c r="K44" s="109"/>
-      <c r="L44" s="104"/>
-      <c r="M44" s="104"/>
+        <v>108</v>
+      </c>
+      <c r="B44" s="112" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="112"/>
+      <c r="D44" s="112"/>
+      <c r="E44" s="109" t="s">
+        <v>87</v>
+      </c>
+      <c r="F44" s="110"/>
+      <c r="G44" s="111"/>
+      <c r="H44" s="109"/>
+      <c r="I44" s="110"/>
+      <c r="J44" s="110"/>
+      <c r="K44" s="111"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="33"/>
     </row>
     <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="18">
         <v>2.1</v>
       </c>
-      <c r="B45" s="105" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="105"/>
-      <c r="D45" s="105"/>
-      <c r="E45" s="105"/>
-      <c r="F45" s="105"/>
-      <c r="G45" s="105"/>
-      <c r="H45" s="105"/>
-      <c r="I45" s="105"/>
-      <c r="J45" s="105"/>
-      <c r="K45" s="105"/>
-      <c r="L45" s="105"/>
-      <c r="M45" s="105"/>
+      <c r="B45" s="112" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="112"/>
+      <c r="D45" s="112"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="112"/>
+      <c r="G45" s="112"/>
+      <c r="H45" s="112"/>
+      <c r="I45" s="112"/>
+      <c r="J45" s="112"/>
+      <c r="K45" s="112"/>
+      <c r="L45" s="112"/>
+      <c r="M45" s="112"/>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B46" s="105" t="s">
-        <v>128</v>
-      </c>
-      <c r="C46" s="105"/>
-      <c r="D46" s="105"/>
-      <c r="E46" s="105" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" s="105"/>
-      <c r="G46" s="105"/>
-      <c r="H46" s="108"/>
-      <c r="I46" s="103"/>
-      <c r="J46" s="103"/>
-      <c r="K46" s="109"/>
-      <c r="L46" s="104"/>
-      <c r="M46" s="104"/>
+        <v>109</v>
+      </c>
+      <c r="B46" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="112"/>
+      <c r="D46" s="112"/>
+      <c r="E46" s="112" t="s">
+        <v>91</v>
+      </c>
+      <c r="F46" s="112"/>
+      <c r="G46" s="112"/>
+      <c r="H46" s="109"/>
+      <c r="I46" s="110"/>
+      <c r="J46" s="110"/>
+      <c r="K46" s="111"/>
+      <c r="L46" s="33"/>
+      <c r="M46" s="33"/>
     </row>
     <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="B47" s="105" t="s">
-        <v>123</v>
-      </c>
-      <c r="C47" s="105"/>
-      <c r="D47" s="105"/>
-      <c r="E47" s="105" t="s">
-        <v>94</v>
-      </c>
-      <c r="F47" s="105"/>
-      <c r="G47" s="105"/>
-      <c r="H47" s="108"/>
-      <c r="I47" s="103"/>
-      <c r="J47" s="103"/>
-      <c r="K47" s="109"/>
-      <c r="L47" s="104"/>
-      <c r="M47" s="104"/>
+        <v>110</v>
+      </c>
+      <c r="B47" s="112" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="112"/>
+      <c r="D47" s="112"/>
+      <c r="E47" s="112" t="s">
+        <v>92</v>
+      </c>
+      <c r="F47" s="112"/>
+      <c r="G47" s="112"/>
+      <c r="H47" s="109"/>
+      <c r="I47" s="110"/>
+      <c r="J47" s="110"/>
+      <c r="K47" s="111"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="33"/>
     </row>
     <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="B48" s="105" t="s">
-        <v>127</v>
-      </c>
-      <c r="C48" s="105"/>
-      <c r="D48" s="105"/>
-      <c r="E48" s="105" t="s">
-        <v>95</v>
-      </c>
-      <c r="F48" s="105"/>
-      <c r="G48" s="105"/>
-      <c r="H48" s="108"/>
-      <c r="I48" s="103"/>
-      <c r="J48" s="103"/>
-      <c r="K48" s="109"/>
-      <c r="L48" s="104"/>
-      <c r="M48" s="104"/>
+        <v>111</v>
+      </c>
+      <c r="B48" s="112" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" s="112"/>
+      <c r="D48" s="112"/>
+      <c r="E48" s="112" t="s">
+        <v>93</v>
+      </c>
+      <c r="F48" s="112"/>
+      <c r="G48" s="112"/>
+      <c r="H48" s="109"/>
+      <c r="I48" s="110"/>
+      <c r="J48" s="110"/>
+      <c r="K48" s="111"/>
+      <c r="L48" s="33"/>
+      <c r="M48" s="33"/>
     </row>
     <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="111">
+      <c r="A49" s="37">
         <v>3</v>
       </c>
-      <c r="B49" s="112" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="112"/>
-      <c r="D49" s="112"/>
-      <c r="E49" s="112"/>
-      <c r="F49" s="112"/>
-      <c r="G49" s="112"/>
-      <c r="H49" s="112"/>
-      <c r="I49" s="112"/>
-      <c r="J49" s="112"/>
-      <c r="K49" s="112"/>
-      <c r="L49" s="112"/>
-      <c r="M49" s="112"/>
+      <c r="B49" s="113" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" s="113"/>
+      <c r="D49" s="113"/>
+      <c r="E49" s="113"/>
+      <c r="F49" s="113"/>
+      <c r="G49" s="113"/>
+      <c r="H49" s="113"/>
+      <c r="I49" s="113"/>
+      <c r="J49" s="113"/>
+      <c r="K49" s="113"/>
+      <c r="L49" s="113"/>
+      <c r="M49" s="113"/>
     </row>
     <row r="50" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="18">
         <v>3.1</v>
       </c>
-      <c r="B50" s="105" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50" s="105"/>
-      <c r="D50" s="105"/>
-      <c r="E50" s="105"/>
-      <c r="F50" s="105"/>
-      <c r="G50" s="105"/>
-      <c r="H50" s="105"/>
-      <c r="I50" s="105"/>
-      <c r="J50" s="105"/>
-      <c r="K50" s="105"/>
-      <c r="L50" s="105"/>
-      <c r="M50" s="105"/>
+      <c r="B50" s="112" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" s="112"/>
+      <c r="D50" s="112"/>
+      <c r="E50" s="112"/>
+      <c r="F50" s="112"/>
+      <c r="G50" s="112"/>
+      <c r="H50" s="112"/>
+      <c r="I50" s="112"/>
+      <c r="J50" s="112"/>
+      <c r="K50" s="112"/>
+      <c r="L50" s="112"/>
+      <c r="M50" s="112"/>
     </row>
     <row r="51" spans="1:13" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B51" s="108" t="s">
-        <v>132</v>
-      </c>
-      <c r="C51" s="103"/>
-      <c r="D51" s="109"/>
-      <c r="E51" s="108" t="s">
-        <v>130</v>
-      </c>
-      <c r="F51" s="103"/>
-      <c r="G51" s="109"/>
-      <c r="H51" s="108"/>
-      <c r="I51" s="103"/>
-      <c r="J51" s="103"/>
-      <c r="K51" s="109"/>
-      <c r="L51" s="104"/>
-      <c r="M51" s="104"/>
+        <v>67</v>
+      </c>
+      <c r="B51" s="109" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="110"/>
+      <c r="D51" s="111"/>
+      <c r="E51" s="109" t="s">
+        <v>126</v>
+      </c>
+      <c r="F51" s="110"/>
+      <c r="G51" s="111"/>
+      <c r="H51" s="109"/>
+      <c r="I51" s="110"/>
+      <c r="J51" s="110"/>
+      <c r="K51" s="111"/>
+      <c r="L51" s="33"/>
+      <c r="M51" s="33"/>
     </row>
     <row r="52" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="18">
         <v>3.2</v>
       </c>
-      <c r="B52" s="105" t="s">
-        <v>117</v>
-      </c>
-      <c r="C52" s="105"/>
-      <c r="D52" s="105"/>
-      <c r="E52" s="105"/>
-      <c r="F52" s="105"/>
-      <c r="G52" s="105"/>
-      <c r="H52" s="105"/>
-      <c r="I52" s="105"/>
-      <c r="J52" s="105"/>
-      <c r="K52" s="105"/>
-      <c r="L52" s="105"/>
-      <c r="M52" s="105"/>
+      <c r="B52" s="112" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" s="112"/>
+      <c r="D52" s="112"/>
+      <c r="E52" s="112"/>
+      <c r="F52" s="112"/>
+      <c r="G52" s="112"/>
+      <c r="H52" s="112"/>
+      <c r="I52" s="112"/>
+      <c r="J52" s="112"/>
+      <c r="K52" s="112"/>
+      <c r="L52" s="112"/>
+      <c r="M52" s="112"/>
     </row>
     <row r="53" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B53" s="108" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" s="103"/>
-      <c r="D53" s="109"/>
-      <c r="E53" s="108" t="s">
-        <v>131</v>
-      </c>
-      <c r="F53" s="103"/>
-      <c r="G53" s="109"/>
-      <c r="H53" s="108"/>
-      <c r="I53" s="103"/>
-      <c r="J53" s="103"/>
-      <c r="K53" s="109"/>
-      <c r="L53" s="104"/>
-      <c r="M53" s="104"/>
+        <v>68</v>
+      </c>
+      <c r="B53" s="109" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="110"/>
+      <c r="D53" s="111"/>
+      <c r="E53" s="109" t="s">
+        <v>127</v>
+      </c>
+      <c r="F53" s="110"/>
+      <c r="G53" s="111"/>
+      <c r="H53" s="109"/>
+      <c r="I53" s="110"/>
+      <c r="J53" s="110"/>
+      <c r="K53" s="111"/>
+      <c r="L53" s="33"/>
+      <c r="M53" s="33"/>
     </row>
     <row r="54" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="18">
         <v>3.3</v>
       </c>
-      <c r="B54" s="105" t="s">
-        <v>54</v>
-      </c>
-      <c r="C54" s="105"/>
-      <c r="D54" s="105"/>
-      <c r="E54" s="105"/>
-      <c r="F54" s="105"/>
-      <c r="G54" s="105"/>
-      <c r="H54" s="105"/>
-      <c r="I54" s="105"/>
-      <c r="J54" s="105"/>
-      <c r="K54" s="105"/>
-      <c r="L54" s="105"/>
-      <c r="M54" s="105"/>
+      <c r="B54" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" s="112"/>
+      <c r="D54" s="112"/>
+      <c r="E54" s="112"/>
+      <c r="F54" s="112"/>
+      <c r="G54" s="112"/>
+      <c r="H54" s="112"/>
+      <c r="I54" s="112"/>
+      <c r="J54" s="112"/>
+      <c r="K54" s="112"/>
+      <c r="L54" s="112"/>
+      <c r="M54" s="112"/>
     </row>
     <row r="55" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B55" s="108" t="s">
-        <v>133</v>
-      </c>
-      <c r="C55" s="103"/>
-      <c r="D55" s="109"/>
-      <c r="E55" s="108" t="s">
-        <v>130</v>
-      </c>
-      <c r="F55" s="103"/>
-      <c r="G55" s="109"/>
-      <c r="H55" s="108"/>
-      <c r="I55" s="103"/>
-      <c r="J55" s="103"/>
-      <c r="K55" s="109"/>
-      <c r="L55" s="104"/>
-      <c r="M55" s="104"/>
+        <v>69</v>
+      </c>
+      <c r="B55" s="109" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="110"/>
+      <c r="D55" s="111"/>
+      <c r="E55" s="109" t="s">
+        <v>126</v>
+      </c>
+      <c r="F55" s="110"/>
+      <c r="G55" s="111"/>
+      <c r="H55" s="109"/>
+      <c r="I55" s="110"/>
+      <c r="J55" s="110"/>
+      <c r="K55" s="111"/>
+      <c r="L55" s="33"/>
+      <c r="M55" s="33"/>
     </row>
     <row r="56" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B56" s="108" t="s">
-        <v>134</v>
-      </c>
-      <c r="C56" s="103"/>
-      <c r="D56" s="109"/>
-      <c r="E56" s="108" t="s">
-        <v>81</v>
-      </c>
-      <c r="F56" s="103"/>
-      <c r="G56" s="109"/>
-      <c r="H56" s="108"/>
-      <c r="I56" s="103"/>
-      <c r="J56" s="103"/>
-      <c r="K56" s="109"/>
-      <c r="L56" s="104"/>
-      <c r="M56" s="104"/>
+        <v>70</v>
+      </c>
+      <c r="B56" s="109" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="110"/>
+      <c r="D56" s="111"/>
+      <c r="E56" s="109" t="s">
+        <v>79</v>
+      </c>
+      <c r="F56" s="110"/>
+      <c r="G56" s="111"/>
+      <c r="H56" s="109"/>
+      <c r="I56" s="110"/>
+      <c r="J56" s="110"/>
+      <c r="K56" s="111"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="33"/>
     </row>
     <row r="57" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="110"/>
-      <c r="B57" s="106"/>
-      <c r="C57" s="106"/>
-      <c r="D57" s="106"/>
-      <c r="E57" s="106"/>
-      <c r="F57" s="106"/>
-      <c r="G57" s="106"/>
-      <c r="H57" s="106"/>
-      <c r="I57" s="106"/>
-      <c r="J57" s="106"/>
-      <c r="K57" s="106"/>
-      <c r="L57" s="106"/>
-      <c r="M57" s="106"/>
+      <c r="A57" s="36"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="34"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="34"/>
+      <c r="K57" s="34"/>
+      <c r="L57" s="34"/>
+      <c r="M57" s="34"/>
     </row>
     <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
@@ -3864,40 +3859,62 @@
     <row r="63" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="128">
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="H55:K55"/>
-    <mergeCell ref="H56:K56"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="H47:K47"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="B26:M26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B50:M50"/>
+    <mergeCell ref="B52:M52"/>
+    <mergeCell ref="B54:M54"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B10:M10"/>
+    <mergeCell ref="B31:M31"/>
+    <mergeCell ref="B41:M41"/>
+    <mergeCell ref="B49:M49"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B21:M21"/>
+    <mergeCell ref="B37:M37"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B45:M45"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="H40:K40"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B44:D44"/>
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="E47:G47"/>
     <mergeCell ref="B48:D48"/>
@@ -3922,18 +3939,17 @@
     <mergeCell ref="E40:G40"/>
     <mergeCell ref="E42:G42"/>
     <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B45:M45"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:K36"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="B26:M26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="H27:K27"/>
     <mergeCell ref="E27:G27"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="H40:K40"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="H22:K22"/>
@@ -3943,55 +3959,34 @@
     <mergeCell ref="H17:K17"/>
     <mergeCell ref="H18:K18"/>
     <mergeCell ref="E18:G18"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="B50:M50"/>
-    <mergeCell ref="B52:M52"/>
-    <mergeCell ref="B54:M54"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B10:M10"/>
-    <mergeCell ref="B31:M31"/>
-    <mergeCell ref="B41:M41"/>
-    <mergeCell ref="B49:M49"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="B16:M16"/>
-    <mergeCell ref="B21:M21"/>
-    <mergeCell ref="B37:M37"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="H55:K55"/>
+    <mergeCell ref="H56:K56"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E46:G46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>